<commit_message>
Added HiSat2 Alignment Performance Analysis
</commit_message>
<xml_diff>
--- a/ComparingMappingRates.xlsx
+++ b/ComparingMappingRates.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>BWA</t>
   </si>
@@ -85,6 +85,9 @@
   <si>
     <t>Overall Mapping Rate</t>
   </si>
+  <si>
+    <t>HiSat2</t>
+  </si>
 </sst>
 </file>
 
@@ -96,6 +99,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -146,9 +150,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="72">
+  <cellStyleXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -230,7 +240,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="72">
+  <cellStyles count="78">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -266,6 +276,9 @@
     <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -301,10 +314,63 @@
     <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -656,16 +722,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H113"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -697,6 +765,9 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -713,7 +784,9 @@
       <c r="D6">
         <v>50.3459</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="E6">
+        <v>36.68</v>
+      </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8">
@@ -729,7 +802,9 @@
       <c r="D7">
         <v>76.837599999999995</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="E7">
+        <v>60.199999999999996</v>
+      </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8">
@@ -746,7 +821,9 @@
       <c r="D8">
         <v>34.736800000000002</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="E8">
+        <v>22.71</v>
+      </c>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8">
@@ -763,7 +840,9 @@
       <c r="D9">
         <v>15.9221</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="E9">
+        <v>6.47</v>
+      </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8">
@@ -780,7 +859,9 @@
       <c r="D10">
         <v>62.138099999999994</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="E10">
+        <v>46.739999999999995</v>
+      </c>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8">
@@ -797,7 +878,9 @@
       <c r="D11">
         <v>40.504300000000001</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="E11">
+        <v>29.65</v>
+      </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8">
@@ -814,7 +897,9 @@
       <c r="D12">
         <v>11.446000000000002</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="E12">
+        <v>3.3000000000000003</v>
+      </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8">
@@ -831,7 +916,9 @@
       <c r="D13">
         <v>32.603400000000001</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="E13">
+        <v>22.55</v>
+      </c>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8">
@@ -848,7 +935,9 @@
       <c r="D14">
         <v>35.641400000000004</v>
       </c>
-      <c r="G14" s="5"/>
+      <c r="E14">
+        <v>22.5</v>
+      </c>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8">
@@ -865,7 +954,9 @@
       <c r="D15">
         <v>83.844799999999992</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="E15">
+        <v>71.89</v>
+      </c>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8">
@@ -882,7 +973,9 @@
       <c r="D16">
         <v>51.314099999999996</v>
       </c>
-      <c r="G16" s="5"/>
+      <c r="E16">
+        <v>39.17</v>
+      </c>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8">
@@ -899,7 +992,9 @@
       <c r="D17">
         <v>34.944199999999995</v>
       </c>
-      <c r="G17" s="5"/>
+      <c r="E17">
+        <v>25.28</v>
+      </c>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8">
@@ -916,7 +1011,9 @@
       <c r="D18">
         <v>49.464000000000006</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="E18">
+        <v>35.68</v>
+      </c>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8">
@@ -933,7 +1030,9 @@
       <c r="D19">
         <v>57.766399999999997</v>
       </c>
-      <c r="G19" s="5"/>
+      <c r="E19">
+        <v>41.85</v>
+      </c>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8">
@@ -950,7 +1049,9 @@
       <c r="D20">
         <v>42.6357</v>
       </c>
-      <c r="G20" s="5"/>
+      <c r="E20">
+        <v>32.04</v>
+      </c>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8">
@@ -967,7 +1068,9 @@
       <c r="D21">
         <v>33.2042</v>
       </c>
-      <c r="G21" s="5"/>
+      <c r="E21">
+        <v>5.99</v>
+      </c>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8">
@@ -984,7 +1087,9 @@
       <c r="D22">
         <v>47.4604</v>
       </c>
-      <c r="G22" s="5"/>
+      <c r="E22">
+        <v>34.47</v>
+      </c>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8">
@@ -1001,7 +1106,9 @@
       <c r="D23">
         <v>56.599800000000002</v>
       </c>
-      <c r="G23" s="5"/>
+      <c r="E23">
+        <v>46.03</v>
+      </c>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8">
@@ -1018,7 +1125,9 @@
       <c r="D24">
         <v>22.278700000000001</v>
       </c>
-      <c r="G24" s="5"/>
+      <c r="E24">
+        <v>11.55</v>
+      </c>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8">
@@ -1035,7 +1144,9 @@
       <c r="D25">
         <v>50.9161</v>
       </c>
-      <c r="G25" s="5"/>
+      <c r="E25">
+        <v>36.730000000000004</v>
+      </c>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8">
@@ -1052,7 +1163,9 @@
       <c r="D26">
         <v>75.6541</v>
       </c>
-      <c r="G26" s="5"/>
+      <c r="E26">
+        <v>59.29</v>
+      </c>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8">
@@ -1069,7 +1182,9 @@
       <c r="D27">
         <v>69.884799999999998</v>
       </c>
-      <c r="G27" s="5"/>
+      <c r="E27">
+        <v>58.589999999999996</v>
+      </c>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8">
@@ -1086,7 +1201,9 @@
       <c r="D28">
         <v>70.047899999999998</v>
       </c>
-      <c r="G28" s="5"/>
+      <c r="E28">
+        <v>54.75</v>
+      </c>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8">
@@ -1103,7 +1220,9 @@
       <c r="D29">
         <v>89.664299999999997</v>
       </c>
-      <c r="G29" s="5"/>
+      <c r="E29">
+        <v>74.429999999999993</v>
+      </c>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8">
@@ -1120,7 +1239,9 @@
       <c r="D30">
         <v>46.304400000000001</v>
       </c>
-      <c r="G30" s="5"/>
+      <c r="E30">
+        <v>36.26</v>
+      </c>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8">
@@ -1137,7 +1258,9 @@
       <c r="D31">
         <v>58.054099999999998</v>
       </c>
-      <c r="G31" s="5"/>
+      <c r="E31">
+        <v>46.589999999999996</v>
+      </c>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8">
@@ -1154,7 +1277,9 @@
       <c r="D32">
         <v>71.886700000000005</v>
       </c>
-      <c r="G32" s="5"/>
+      <c r="E32">
+        <v>56.07</v>
+      </c>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8">
@@ -1171,7 +1296,9 @@
       <c r="D33">
         <v>93.003599999999992</v>
       </c>
-      <c r="G33" s="5"/>
+      <c r="E33">
+        <v>83.12</v>
+      </c>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8">
@@ -1188,7 +1315,9 @@
       <c r="D34">
         <v>77.066400000000002</v>
       </c>
-      <c r="G34" s="5"/>
+      <c r="E34">
+        <v>61.309999999999995</v>
+      </c>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8">
@@ -1205,7 +1334,9 @@
       <c r="D35">
         <v>44.0702</v>
       </c>
-      <c r="G35" s="5"/>
+      <c r="E35">
+        <v>34.270000000000003</v>
+      </c>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8">
@@ -1222,7 +1353,9 @@
       <c r="D36">
         <v>28.579599999999999</v>
       </c>
-      <c r="G36" s="5"/>
+      <c r="E36">
+        <v>19.850000000000001</v>
+      </c>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8">
@@ -1239,7 +1372,9 @@
       <c r="D37">
         <v>85.392399999999995</v>
       </c>
-      <c r="G37" s="5"/>
+      <c r="E37">
+        <v>66.320000000000007</v>
+      </c>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8">
@@ -1256,7 +1391,9 @@
       <c r="D38">
         <v>59.728300000000004</v>
       </c>
-      <c r="G38" s="5"/>
+      <c r="E38">
+        <v>47.08</v>
+      </c>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8">
@@ -1273,7 +1410,9 @@
       <c r="D39">
         <v>42.130899999999997</v>
       </c>
-      <c r="G39" s="5"/>
+      <c r="E39">
+        <v>33.21</v>
+      </c>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8">
@@ -1290,7 +1429,9 @@
       <c r="D40">
         <v>78.256599999999992</v>
       </c>
-      <c r="G40" s="5"/>
+      <c r="E40">
+        <v>62.91</v>
+      </c>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8">
@@ -1307,7 +1448,9 @@
       <c r="D41">
         <v>72.831699999999998</v>
       </c>
-      <c r="G41" s="5"/>
+      <c r="E41">
+        <v>59.870000000000005</v>
+      </c>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8">
@@ -1324,7 +1467,9 @@
       <c r="D42">
         <v>32.090299999999999</v>
       </c>
-      <c r="G42" s="5"/>
+      <c r="E42">
+        <v>19.170000000000002</v>
+      </c>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8">
@@ -1341,7 +1486,9 @@
       <c r="D43">
         <v>65.097200000000001</v>
       </c>
-      <c r="G43" s="5"/>
+      <c r="E43">
+        <v>52.66</v>
+      </c>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8">
@@ -1358,7 +1505,9 @@
       <c r="D44">
         <v>68.919600000000003</v>
       </c>
-      <c r="G44" s="5"/>
+      <c r="E44">
+        <v>56.04</v>
+      </c>
       <c r="H44" s="5"/>
     </row>
     <row r="45" spans="1:8">
@@ -1375,7 +1524,9 @@
       <c r="D45">
         <v>67.530599999999993</v>
       </c>
-      <c r="G45" s="5"/>
+      <c r="E45">
+        <v>53</v>
+      </c>
       <c r="H45" s="5"/>
     </row>
     <row r="46" spans="1:8">
@@ -1392,7 +1543,9 @@
       <c r="D46">
         <v>71.528599999999997</v>
       </c>
-      <c r="G46" s="5"/>
+      <c r="E46">
+        <v>56.410000000000004</v>
+      </c>
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:8">
@@ -1409,7 +1562,9 @@
       <c r="D47">
         <v>36.608600000000003</v>
       </c>
-      <c r="G47" s="5"/>
+      <c r="E47">
+        <v>21.34</v>
+      </c>
       <c r="H47" s="5"/>
     </row>
     <row r="48" spans="1:8">
@@ -1426,7 +1581,9 @@
       <c r="D48">
         <v>74.530300000000011</v>
       </c>
-      <c r="G48" s="5"/>
+      <c r="E48">
+        <v>59.51</v>
+      </c>
       <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:8">
@@ -1443,7 +1600,9 @@
       <c r="D49">
         <v>76.920400000000001</v>
       </c>
-      <c r="G49" s="5"/>
+      <c r="E49">
+        <v>62.019999999999996</v>
+      </c>
       <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:8">
@@ -1460,7 +1619,9 @@
       <c r="D50">
         <v>62.032299999999992</v>
       </c>
-      <c r="G50" s="5"/>
+      <c r="E50">
+        <v>45.59</v>
+      </c>
       <c r="H50" s="5"/>
     </row>
     <row r="51" spans="1:8">
@@ -1477,7 +1638,9 @@
       <c r="D51">
         <v>83.250100000000003</v>
       </c>
-      <c r="G51" s="5"/>
+      <c r="E51">
+        <v>65.149999999999991</v>
+      </c>
       <c r="H51" s="5"/>
     </row>
     <row r="52" spans="1:8">
@@ -1494,7 +1657,9 @@
       <c r="D52">
         <v>21.2057</v>
       </c>
-      <c r="G52" s="5"/>
+      <c r="E52">
+        <v>7.2499999999999991</v>
+      </c>
       <c r="H52" s="5"/>
     </row>
     <row r="53" spans="1:8">
@@ -1511,7 +1676,9 @@
       <c r="D53">
         <v>81.769599999999997</v>
       </c>
-      <c r="G53" s="5"/>
+      <c r="E53">
+        <v>64.58</v>
+      </c>
       <c r="H53" s="5"/>
     </row>
     <row r="54" spans="1:8">
@@ -1528,7 +1695,9 @@
       <c r="D54">
         <v>57.384900000000002</v>
       </c>
-      <c r="G54" s="5"/>
+      <c r="E54">
+        <v>43.76</v>
+      </c>
       <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:8">
@@ -1545,7 +1714,9 @@
       <c r="D55">
         <v>19.122399999999999</v>
       </c>
-      <c r="G55" s="5"/>
+      <c r="E55">
+        <v>7.21</v>
+      </c>
       <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:8">
@@ -1562,7 +1733,9 @@
       <c r="D56">
         <v>61.396499999999996</v>
       </c>
-      <c r="G56" s="5"/>
+      <c r="E56">
+        <v>43.89</v>
+      </c>
       <c r="H56" s="5"/>
     </row>
     <row r="57" spans="1:8">
@@ -1579,7 +1752,9 @@
       <c r="D57">
         <v>58.503300000000003</v>
       </c>
-      <c r="G57" s="5"/>
+      <c r="E57">
+        <v>44.92</v>
+      </c>
       <c r="H57" s="5"/>
     </row>
     <row r="58" spans="1:8">
@@ -1596,7 +1771,9 @@
       <c r="D58">
         <v>26.574399999999997</v>
       </c>
-      <c r="G58" s="5"/>
+      <c r="E58">
+        <v>15.989999999999998</v>
+      </c>
       <c r="H58" s="5"/>
     </row>
     <row r="59" spans="1:8">
@@ -1613,7 +1790,9 @@
       <c r="D59">
         <v>19.318200000000001</v>
       </c>
-      <c r="G59" s="5"/>
+      <c r="E59">
+        <v>8.5500000000000007</v>
+      </c>
       <c r="H59" s="5"/>
     </row>
     <row r="60" spans="1:8">
@@ -1630,7 +1809,9 @@
       <c r="D60">
         <v>24.983699999999999</v>
       </c>
-      <c r="G60" s="5"/>
+      <c r="E60">
+        <v>11.01</v>
+      </c>
       <c r="H60" s="5"/>
     </row>
     <row r="61" spans="1:8">
@@ -1647,7 +1828,9 @@
       <c r="D61">
         <v>40.630099999999999</v>
       </c>
-      <c r="G61" s="5"/>
+      <c r="E61">
+        <v>28.24</v>
+      </c>
       <c r="H61" s="5"/>
     </row>
     <row r="62" spans="1:8">
@@ -1664,7 +1847,9 @@
       <c r="D62">
         <v>83.577399999999997</v>
       </c>
-      <c r="G62" s="5"/>
+      <c r="E62">
+        <v>65.33</v>
+      </c>
       <c r="H62" s="5"/>
     </row>
     <row r="63" spans="1:8">
@@ -1681,7 +1866,9 @@
       <c r="D63">
         <v>14.8207</v>
       </c>
-      <c r="G63" s="5"/>
+      <c r="E63">
+        <v>1.01</v>
+      </c>
       <c r="H63" s="5"/>
     </row>
     <row r="64" spans="1:8">
@@ -1698,7 +1885,9 @@
       <c r="D64">
         <v>58.482599999999998</v>
       </c>
-      <c r="G64" s="5"/>
+      <c r="E64">
+        <v>42.27</v>
+      </c>
       <c r="H64" s="5"/>
     </row>
     <row r="65" spans="1:8">
@@ -1715,7 +1904,9 @@
       <c r="D65">
         <v>65.6447</v>
       </c>
-      <c r="G65" s="5"/>
+      <c r="E65">
+        <v>52.2</v>
+      </c>
       <c r="H65" s="5"/>
     </row>
     <row r="66" spans="1:8">
@@ -1732,7 +1923,9 @@
       <c r="D66">
         <v>32.414000000000001</v>
       </c>
-      <c r="G66" s="5"/>
+      <c r="E66">
+        <v>18.149999999999999</v>
+      </c>
       <c r="H66" s="5"/>
     </row>
     <row r="67" spans="1:8">
@@ -1749,7 +1942,9 @@
       <c r="D67">
         <v>68.409199999999998</v>
       </c>
-      <c r="G67" s="5"/>
+      <c r="E67">
+        <v>52.73</v>
+      </c>
       <c r="H67" s="5"/>
     </row>
     <row r="68" spans="1:8">
@@ -1766,7 +1961,9 @@
       <c r="D68">
         <v>11.2774</v>
       </c>
-      <c r="G68" s="5"/>
+      <c r="E68">
+        <v>2.0699999999999998</v>
+      </c>
       <c r="H68" s="5"/>
     </row>
     <row r="69" spans="1:8">
@@ -1783,7 +1980,9 @@
       <c r="D69">
         <v>31.270599999999998</v>
       </c>
-      <c r="G69" s="5"/>
+      <c r="E69">
+        <v>15.4</v>
+      </c>
       <c r="H69" s="5"/>
     </row>
     <row r="70" spans="1:8">
@@ -1800,7 +1999,9 @@
       <c r="D70">
         <v>20.973800000000001</v>
       </c>
-      <c r="G70" s="5"/>
+      <c r="E70">
+        <v>12.36</v>
+      </c>
       <c r="H70" s="5"/>
     </row>
     <row r="71" spans="1:8">
@@ -1817,7 +2018,9 @@
       <c r="D71">
         <v>43.333300000000001</v>
       </c>
-      <c r="G71" s="5"/>
+      <c r="E71">
+        <v>30</v>
+      </c>
       <c r="H71" s="5"/>
     </row>
     <row r="72" spans="1:8">
@@ -1834,7 +2037,9 @@
       <c r="D72">
         <v>85.103799999999993</v>
       </c>
-      <c r="G72" s="5"/>
+      <c r="E72">
+        <v>70.39</v>
+      </c>
       <c r="H72" s="5"/>
     </row>
     <row r="73" spans="1:8">
@@ -1851,7 +2056,9 @@
       <c r="D73">
         <v>61.444699999999997</v>
       </c>
-      <c r="G73" s="5"/>
+      <c r="E73">
+        <v>45.26</v>
+      </c>
       <c r="H73" s="5"/>
     </row>
     <row r="74" spans="1:8">
@@ -1868,7 +2075,9 @@
       <c r="D74">
         <v>61.885199999999998</v>
       </c>
-      <c r="G74" s="5"/>
+      <c r="E74">
+        <v>44.67</v>
+      </c>
       <c r="H74" s="5"/>
     </row>
     <row r="75" spans="1:8">
@@ -1885,7 +2094,9 @@
       <c r="D75">
         <v>45.898000000000003</v>
       </c>
-      <c r="G75" s="5"/>
+      <c r="E75">
+        <v>29.49</v>
+      </c>
       <c r="H75" s="5"/>
     </row>
     <row r="76" spans="1:8">
@@ -1902,7 +2113,9 @@
       <c r="D76">
         <v>55.645199999999996</v>
       </c>
-      <c r="G76" s="5"/>
+      <c r="E76">
+        <v>44.09</v>
+      </c>
       <c r="H76" s="5"/>
     </row>
     <row r="77" spans="1:8">
@@ -1919,7 +2132,9 @@
       <c r="D77">
         <v>39.4345</v>
       </c>
-      <c r="G77" s="5"/>
+      <c r="E77">
+        <v>22.400000000000002</v>
+      </c>
       <c r="H77" s="5"/>
     </row>
     <row r="78" spans="1:8">
@@ -1936,7 +2151,9 @@
       <c r="D78">
         <v>70.129599999999996</v>
       </c>
-      <c r="G78" s="5"/>
+      <c r="E78">
+        <v>55.63</v>
+      </c>
       <c r="H78" s="5"/>
     </row>
     <row r="79" spans="1:8">
@@ -1953,7 +2170,9 @@
       <c r="D79">
         <v>72.779300000000006</v>
       </c>
-      <c r="G79" s="5"/>
+      <c r="E79">
+        <v>59.589999999999996</v>
+      </c>
       <c r="H79" s="5"/>
     </row>
     <row r="80" spans="1:8">
@@ -1970,7 +2189,9 @@
       <c r="D80">
         <v>70.95</v>
       </c>
-      <c r="G80" s="5"/>
+      <c r="E80">
+        <v>52.55</v>
+      </c>
       <c r="H80" s="5"/>
     </row>
     <row r="81" spans="1:8">
@@ -1987,7 +2208,9 @@
       <c r="D81">
         <v>43.5411</v>
       </c>
-      <c r="G81" s="5"/>
+      <c r="E81">
+        <v>27.68</v>
+      </c>
       <c r="H81" s="5"/>
     </row>
     <row r="82" spans="1:8">
@@ -2004,7 +2227,9 @@
       <c r="D82">
         <v>61.690100000000001</v>
       </c>
-      <c r="G82" s="5"/>
+      <c r="E82">
+        <v>44.51</v>
+      </c>
       <c r="H82" s="5"/>
     </row>
     <row r="83" spans="1:8">
@@ -2021,7 +2246,9 @@
       <c r="D83">
         <v>71.123000000000005</v>
       </c>
-      <c r="G83" s="5"/>
+      <c r="E83">
+        <v>51.82</v>
+      </c>
       <c r="H83" s="5"/>
     </row>
     <row r="84" spans="1:8">
@@ -2038,7 +2265,9 @@
       <c r="D84">
         <v>90.950100000000006</v>
       </c>
-      <c r="G84" s="5"/>
+      <c r="E84">
+        <v>73.94</v>
+      </c>
       <c r="H84" s="5"/>
     </row>
     <row r="85" spans="1:8">
@@ -2055,7 +2284,9 @@
       <c r="D85">
         <v>58.569000000000003</v>
       </c>
-      <c r="G85" s="5"/>
+      <c r="E85">
+        <v>45.08</v>
+      </c>
       <c r="H85" s="5"/>
     </row>
     <row r="86" spans="1:8">
@@ -2072,7 +2303,9 @@
       <c r="D86">
         <v>48.148099999999999</v>
       </c>
-      <c r="G86" s="5"/>
+      <c r="E86">
+        <v>33.33</v>
+      </c>
       <c r="H86" s="5"/>
     </row>
     <row r="87" spans="1:8">
@@ -2089,7 +2322,9 @@
       <c r="D87">
         <v>45.794200000000004</v>
       </c>
-      <c r="G87" s="5"/>
+      <c r="E87">
+        <v>30.819999999999997</v>
+      </c>
       <c r="H87" s="5"/>
     </row>
     <row r="88" spans="1:8">
@@ -2106,7 +2341,9 @@
       <c r="D88">
         <v>49.524699999999996</v>
       </c>
-      <c r="G88" s="5"/>
+      <c r="E88">
+        <v>34.150000000000006</v>
+      </c>
       <c r="H88" s="5"/>
     </row>
     <row r="89" spans="1:8">
@@ -2123,7 +2360,9 @@
       <c r="D89">
         <v>17.3066</v>
       </c>
-      <c r="G89" s="5"/>
+      <c r="E89">
+        <v>10.5</v>
+      </c>
       <c r="H89" s="5"/>
     </row>
     <row r="90" spans="1:8">
@@ -2140,7 +2379,9 @@
       <c r="D90">
         <v>47.206600000000002</v>
       </c>
-      <c r="G90" s="5"/>
+      <c r="E90">
+        <v>30.2</v>
+      </c>
       <c r="H90" s="5"/>
     </row>
     <row r="91" spans="1:8">
@@ -2157,7 +2398,9 @@
       <c r="D91">
         <v>56.125100000000003</v>
       </c>
-      <c r="G91" s="5"/>
+      <c r="E91">
+        <v>39.119999999999997</v>
+      </c>
       <c r="H91" s="5"/>
     </row>
     <row r="92" spans="1:8">
@@ -2174,7 +2417,9 @@
       <c r="D92">
         <v>18.6645</v>
       </c>
-      <c r="G92" s="5"/>
+      <c r="E92">
+        <v>9.94</v>
+      </c>
       <c r="H92" s="5"/>
     </row>
     <row r="93" spans="1:8">
@@ -2191,7 +2436,9 @@
       <c r="D93">
         <v>44.814100000000003</v>
       </c>
-      <c r="G93" s="5"/>
+      <c r="E93">
+        <v>31.31</v>
+      </c>
       <c r="H93" s="5"/>
     </row>
     <row r="94" spans="1:8">
@@ -2208,7 +2455,9 @@
       <c r="D94">
         <v>51.166599999999995</v>
       </c>
-      <c r="G94" s="5"/>
+      <c r="E94">
+        <v>41.38</v>
+      </c>
       <c r="H94" s="5"/>
     </row>
     <row r="95" spans="1:8">
@@ -2225,7 +2474,9 @@
       <c r="D95">
         <v>58.241299999999995</v>
       </c>
-      <c r="G95" s="5"/>
+      <c r="E95">
+        <v>39.94</v>
+      </c>
       <c r="H95" s="5"/>
     </row>
     <row r="96" spans="1:8">
@@ -2242,7 +2493,9 @@
       <c r="D96">
         <v>41.842600000000004</v>
       </c>
-      <c r="G96" s="5"/>
+      <c r="E96">
+        <v>19.61</v>
+      </c>
       <c r="H96" s="5"/>
     </row>
     <row r="97" spans="1:8">
@@ -2259,7 +2512,9 @@
       <c r="D97">
         <v>29.884</v>
       </c>
-      <c r="G97" s="5"/>
+      <c r="E97">
+        <v>20.599999999999998</v>
+      </c>
       <c r="H97" s="5"/>
     </row>
     <row r="98" spans="1:8">
@@ -2276,7 +2531,9 @@
       <c r="D98">
         <v>24.455099999999998</v>
       </c>
-      <c r="G98" s="5"/>
+      <c r="E98">
+        <v>11.959999999999999</v>
+      </c>
       <c r="H98" s="5"/>
     </row>
     <row r="99" spans="1:8">
@@ -2293,7 +2550,9 @@
       <c r="D99">
         <v>82.637600000000006</v>
       </c>
-      <c r="G99" s="5"/>
+      <c r="E99">
+        <v>65.64</v>
+      </c>
       <c r="H99" s="5"/>
     </row>
     <row r="100" spans="1:8">
@@ -2310,7 +2569,9 @@
       <c r="D100">
         <v>63.199199999999998</v>
       </c>
-      <c r="G100" s="5"/>
+      <c r="E100">
+        <v>45.26</v>
+      </c>
       <c r="H100" s="5"/>
     </row>
     <row r="101" spans="1:8">
@@ -2327,7 +2588,9 @@
       <c r="D101">
         <v>57.518299999999996</v>
       </c>
-      <c r="G101" s="5"/>
+      <c r="E101">
+        <v>41.21</v>
+      </c>
       <c r="H101" s="5"/>
     </row>
     <row r="105" spans="1:8">
@@ -2339,13 +2602,17 @@
         <v>82</v>
       </c>
       <c r="C105">
-        <f t="shared" ref="C105:D105" si="2">COUNTIF(C6:C101, "&gt;=25")</f>
+        <f t="shared" ref="C105:E105" si="2">COUNTIF(C6:C101, "&gt;=25")</f>
         <v>60</v>
       </c>
       <c r="D105">
         <f t="shared" si="2"/>
         <v>83</v>
       </c>
+      <c r="E105">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
     </row>
     <row r="106" spans="1:8">
       <c r="A106" t="s">
@@ -2356,13 +2623,17 @@
         <v>52</v>
       </c>
       <c r="C106">
-        <f t="shared" ref="C106:D106" si="3">COUNTIF(C6:C101, "&gt;=50")</f>
+        <f t="shared" ref="C106:E106" si="3">COUNTIF(C6:C101, "&gt;=50")</f>
         <v>9</v>
       </c>
       <c r="D106">
         <f t="shared" si="3"/>
         <v>53</v>
       </c>
+      <c r="E106">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
     </row>
     <row r="107" spans="1:8">
       <c r="A107" t="s">
@@ -2373,13 +2644,17 @@
         <v>15</v>
       </c>
       <c r="C107">
-        <f t="shared" ref="C107:D107" si="4">COUNTIF(C6:C101, "&gt;=75")</f>
+        <f t="shared" ref="C107:E107" si="4">COUNTIF(C6:C101, "&gt;=75")</f>
         <v>1</v>
       </c>
       <c r="D107">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
+      <c r="E107">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="108" spans="1:8">
       <c r="A108" t="s">
@@ -2390,13 +2665,17 @@
         <v>10</v>
       </c>
       <c r="C108">
-        <f t="shared" ref="C108:D108" si="5">COUNTIF(C7:C102, "&gt;=80")</f>
+        <f t="shared" ref="C108:E108" si="5">COUNTIF(C7:C102, "&gt;=80")</f>
         <v>0</v>
       </c>
       <c r="D108">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
+      <c r="E108">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="109" spans="1:8">
       <c r="A109" t="s">
@@ -2407,13 +2686,17 @@
         <v>3</v>
       </c>
       <c r="C109">
-        <f t="shared" ref="C109:D109" si="6">COUNTIF(C6:C101, "&gt;=90")</f>
+        <f t="shared" ref="C109:E109" si="6">COUNTIF(C6:C101, "&gt;=90")</f>
         <v>0</v>
       </c>
       <c r="D109">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
+      <c r="E109">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="111" spans="1:8">
       <c r="A111" t="s">
@@ -2428,6 +2711,9 @@
       <c r="D111" s="1">
         <v>388233</v>
       </c>
+      <c r="E111" s="1">
+        <v>267870</v>
+      </c>
     </row>
     <row r="112" spans="1:8">
       <c r="A112" t="s">
@@ -2442,8 +2728,11 @@
       <c r="D112" s="6">
         <v>835683.4930836308</v>
       </c>
-    </row>
-    <row r="113" spans="1:4">
+      <c r="E112" s="6">
+        <v>835683</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
         <v>15</v>
       </c>
@@ -2459,15 +2748,19 @@
         <f>D111/D112</f>
         <v>0.46456942516291594</v>
       </c>
+      <c r="E113" s="7">
+        <f>E111/E112</f>
+        <v>0.32054020483843754</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B114:B1048576 D110:E110 A111:A113 B5:E109 F5">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="B114:B1048576 D110:F110 A111:A113 G5 B5:F109">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E111 C114:E1048576 D112:E113">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="F111 C114:F1048576 D112:F113">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2483,10 +2776,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M98"/>
+  <dimension ref="A2:S98"/>
   <sheetViews>
-    <sheetView topLeftCell="C86" workbookViewId="0">
-      <selection activeCell="G115" sqref="G115"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:S98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2496,7 +2789,7 @@
     <col min="6" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>3002</v>
       </c>
@@ -2527,8 +2820,22 @@
         <f>J2*1/K2</f>
         <v>5926.9970345152242</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="O2" s="5">
+        <v>0.36680000000000001</v>
+      </c>
+      <c r="P2">
+        <f>O2*100</f>
+        <v>36.68</v>
+      </c>
+      <c r="Q2">
+        <v>5927</v>
+      </c>
+      <c r="R2">
+        <f>Q2*O2</f>
+        <v>2174.0236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>20501</v>
       </c>
@@ -2559,8 +2866,22 @@
         <f t="shared" ref="L3:L66" si="2">J3*1/K3</f>
         <v>25903.984507584832</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="O3" s="5">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P66" si="3">O3*100</f>
+        <v>60.199999999999996</v>
+      </c>
+      <c r="Q3">
+        <v>25904</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R66" si="4">Q3*O3</f>
+        <v>15594.207999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>626</v>
       </c>
@@ -2591,8 +2912,22 @@
         <f t="shared" si="2"/>
         <v>1805.0021878814398</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="O4" s="5">
+        <v>0.2271</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="3"/>
+        <v>22.71</v>
+      </c>
+      <c r="Q4">
+        <v>1805</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="4"/>
+        <v>409.91550000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>991</v>
       </c>
@@ -2623,8 +2958,22 @@
         <f t="shared" si="2"/>
         <v>7141.0178305625514</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="O5" s="5">
+        <v>6.4699999999999994E-2</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="3"/>
+        <v>6.47</v>
+      </c>
+      <c r="Q5">
+        <v>7141</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="4"/>
+        <v>462.02269999999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>5390</v>
       </c>
@@ -2655,8 +3004,22 @@
         <f t="shared" si="2"/>
         <v>8325.005109586551</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="O6" s="5">
+        <v>0.46739999999999998</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="3"/>
+        <v>46.739999999999995</v>
+      </c>
+      <c r="Q6">
+        <v>8325</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="4"/>
+        <v>3891.105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>997</v>
       </c>
@@ -2687,8 +3050,22 @@
         <f t="shared" si="2"/>
         <v>2458.9981804401014</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="O7" s="5">
+        <v>0.29649999999999999</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="3"/>
+        <v>29.65</v>
+      </c>
+      <c r="Q7">
+        <v>2459</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="4"/>
+        <v>729.09349999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>233</v>
       </c>
@@ -2719,8 +3096,22 @@
         <f t="shared" si="2"/>
         <v>2455.0061156735978</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="O8" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="3"/>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="Q8">
+        <v>2455</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="4"/>
+        <v>81.015000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>1380</v>
       </c>
@@ -2751,8 +3142,22 @@
         <f t="shared" si="2"/>
         <v>4474.9934055957356</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="O9" s="5">
+        <v>0.22550000000000001</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="3"/>
+        <v>22.55</v>
+      </c>
+      <c r="Q9">
+        <v>4475</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="4"/>
+        <v>1009.1125000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>798</v>
       </c>
@@ -2783,8 +3188,22 @@
         <f t="shared" si="2"/>
         <v>2252.9979181513631</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="O10" s="5">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="3"/>
+        <v>22.5</v>
+      </c>
+      <c r="Q10">
+        <v>2253</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="4"/>
+        <v>506.92500000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>4038</v>
       </c>
@@ -2815,8 +3234,22 @@
         <f t="shared" si="2"/>
         <v>4692.0023662767398</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="O11" s="5">
+        <v>0.71889999999999998</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="3"/>
+        <v>71.89</v>
+      </c>
+      <c r="Q11">
+        <v>4692</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="4"/>
+        <v>3373.0787999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>833</v>
       </c>
@@ -2847,8 +3280,22 @@
         <f t="shared" si="2"/>
         <v>1598.0013290693983</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="O12" s="5">
+        <v>0.39169999999999999</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="3"/>
+        <v>39.17</v>
+      </c>
+      <c r="Q12">
+        <v>1598</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="4"/>
+        <v>625.9366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>643</v>
       </c>
@@ -2879,8 +3326,22 @@
         <f t="shared" si="2"/>
         <v>1883.0020432575363</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="O13" s="5">
+        <v>0.25280000000000002</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="3"/>
+        <v>25.28</v>
+      </c>
+      <c r="Q13">
+        <v>1883</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="4"/>
+        <v>476.02240000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>1622</v>
       </c>
@@ -2911,8 +3372,22 @@
         <f t="shared" si="2"/>
         <v>3265.0008086689309</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="O14" s="5">
+        <v>0.35680000000000001</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="3"/>
+        <v>35.68</v>
+      </c>
+      <c r="Q14">
+        <v>3265</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="4"/>
+        <v>1164.952</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>454</v>
       </c>
@@ -2943,8 +3418,22 @@
         <f t="shared" si="2"/>
         <v>778.99955683580777</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="O15" s="5">
+        <v>0.41849999999999998</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="3"/>
+        <v>41.85</v>
+      </c>
+      <c r="Q15">
+        <v>779</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="4"/>
+        <v>326.01150000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>674</v>
       </c>
@@ -2975,8 +3464,22 @@
         <f t="shared" si="2"/>
         <v>1547.9985082923465</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="O16" s="5">
+        <v>0.32040000000000002</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="3"/>
+        <v>32.04</v>
+      </c>
+      <c r="Q16">
+        <v>1548</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="4"/>
+        <v>495.97920000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17">
         <v>3273</v>
       </c>
@@ -3007,8 +3510,22 @@
         <f t="shared" si="2"/>
         <v>11878.015431782725</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="O17" s="5">
+        <v>5.9900000000000002E-2</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="3"/>
+        <v>5.99</v>
+      </c>
+      <c r="Q17">
+        <v>11878</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="4"/>
+        <v>711.49220000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18">
         <v>1727</v>
       </c>
@@ -3039,8 +3556,22 @@
         <f t="shared" si="2"/>
         <v>3603.0037673513075</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="O18" s="5">
+        <v>0.34470000000000001</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="3"/>
+        <v>34.47</v>
+      </c>
+      <c r="Q18">
+        <v>3603</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="4"/>
+        <v>1241.9540999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19">
         <v>1364</v>
       </c>
@@ -3071,8 +3602,22 @@
         <f t="shared" si="2"/>
         <v>2394.0013922310682</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="O19" s="5">
+        <v>0.46029999999999999</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="3"/>
+        <v>46.03</v>
+      </c>
+      <c r="Q19">
+        <v>2394</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="4"/>
+        <v>1101.9582</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20">
         <v>1051</v>
       </c>
@@ -3103,8 +3648,22 @@
         <f t="shared" si="2"/>
         <v>5116.99515680897</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="O20" s="5">
+        <v>0.11550000000000001</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="3"/>
+        <v>11.55</v>
+      </c>
+      <c r="Q20">
+        <v>5117</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="4"/>
+        <v>591.01350000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21">
         <v>1205</v>
       </c>
@@ -3135,8 +3694,22 @@
         <f t="shared" si="2"/>
         <v>2346.9982971987251</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="O21" s="5">
+        <v>0.36730000000000002</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="3"/>
+        <v>36.730000000000004</v>
+      </c>
+      <c r="Q21">
+        <v>2347</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="4"/>
+        <v>862.05310000000009</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22">
         <v>2515</v>
       </c>
@@ -3167,8 +3740,22 @@
         <f t="shared" si="2"/>
         <v>3134.0006688335461</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="O22" s="5">
+        <v>0.59289999999999998</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="3"/>
+        <v>59.29</v>
+      </c>
+      <c r="Q22">
+        <v>3134</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="4"/>
+        <v>1858.1486</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23">
         <v>2908</v>
       </c>
@@ -3199,8 +3786,22 @@
         <f t="shared" si="2"/>
         <v>4081.0018773753377</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="O23" s="5">
+        <v>0.58589999999999998</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="3"/>
+        <v>58.589999999999996</v>
+      </c>
+      <c r="Q23">
+        <v>4081</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="4"/>
+        <v>2391.0578999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24">
         <v>1805</v>
       </c>
@@ -3231,8 +3832,22 @@
         <f t="shared" si="2"/>
         <v>2504.0008337152149</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="O24" s="5">
+        <v>0.54749999999999999</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="3"/>
+        <v>54.75</v>
+      </c>
+      <c r="Q24">
+        <v>2504</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="4"/>
+        <v>1370.94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25">
         <v>4618</v>
       </c>
@@ -3263,8 +3878,22 @@
         <f t="shared" si="2"/>
         <v>4914.9996152314807</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="O25" s="5">
+        <v>0.74429999999999996</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="3"/>
+        <v>74.429999999999993</v>
+      </c>
+      <c r="Q25">
+        <v>4915</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="4"/>
+        <v>3658.2345</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26">
         <v>3207</v>
       </c>
@@ -3295,8 +3924,22 @@
         <f t="shared" si="2"/>
         <v>6642.9972097684022</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="O26" s="5">
+        <v>0.36259999999999998</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="3"/>
+        <v>36.26</v>
+      </c>
+      <c r="Q26">
+        <v>6643</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="4"/>
+        <v>2408.7518</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27">
         <v>2734</v>
       </c>
@@ -3327,8 +3970,22 @@
         <f t="shared" si="2"/>
         <v>4624.9963396211469</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="O27" s="5">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="3"/>
+        <v>46.589999999999996</v>
+      </c>
+      <c r="Q27">
+        <v>4625</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="4"/>
+        <v>2154.7874999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28">
         <v>1405</v>
       </c>
@@ -3359,8 +4016,22 @@
         <f t="shared" si="2"/>
         <v>1870.999781600769</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="O28" s="5">
+        <v>0.56069999999999998</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="3"/>
+        <v>56.07</v>
+      </c>
+      <c r="Q28">
+        <v>1871</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="4"/>
+        <v>1049.0697</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29">
         <v>17143</v>
       </c>
@@ -3391,8 +4062,22 @@
         <f t="shared" si="2"/>
         <v>17851.997126992934</v>
       </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="O29" s="5">
+        <v>0.83120000000000005</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="3"/>
+        <v>83.12</v>
+      </c>
+      <c r="Q29">
+        <v>17852</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="4"/>
+        <v>14838.582400000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30">
         <v>9991</v>
       </c>
@@ -3423,8 +4108,22 @@
         <f t="shared" si="2"/>
         <v>12449.005013858179</v>
       </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="O30" s="5">
+        <v>0.61309999999999998</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="3"/>
+        <v>61.309999999999995</v>
+      </c>
+      <c r="Q30">
+        <v>12449</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="4"/>
+        <v>7632.4818999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31">
         <v>1606</v>
       </c>
@@ -3455,8 +4154,22 @@
         <f t="shared" si="2"/>
         <v>3591.9964057344873</v>
       </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="O31" s="5">
+        <v>0.3427</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="3"/>
+        <v>34.270000000000003</v>
+      </c>
+      <c r="Q31">
+        <v>3592</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="4"/>
+        <v>1230.9784</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32">
         <v>497</v>
       </c>
@@ -3487,8 +4200,22 @@
         <f>J32*1/K32</f>
         <v>1752.9986423882769</v>
       </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="O32" s="5">
+        <v>0.19850000000000001</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="3"/>
+        <v>19.850000000000001</v>
+      </c>
+      <c r="Q32">
+        <v>1753</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="4"/>
+        <v>347.97050000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33">
         <v>11077</v>
       </c>
@@ -3519,8 +4246,22 @@
         <f t="shared" si="2"/>
         <v>12473.006965491073</v>
       </c>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="O33" s="5">
+        <v>0.66320000000000001</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="3"/>
+        <v>66.320000000000007</v>
+      </c>
+      <c r="Q33">
+        <v>12473</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="4"/>
+        <v>8272.0936000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34">
         <v>3720</v>
       </c>
@@ -3551,8 +4292,22 @@
         <f t="shared" si="2"/>
         <v>5961.9979138867166</v>
       </c>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="O34" s="5">
+        <v>0.4708</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="3"/>
+        <v>47.08</v>
+      </c>
+      <c r="Q34">
+        <v>5962</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="4"/>
+        <v>2806.9096</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
       <c r="A35">
         <v>1989</v>
       </c>
@@ -3583,8 +4338,22 @@
         <f t="shared" si="2"/>
         <v>4721.0005008200633</v>
       </c>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="O35" s="5">
+        <v>0.33210000000000001</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="3"/>
+        <v>33.21</v>
+      </c>
+      <c r="Q35">
+        <v>4721</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="4"/>
+        <v>1567.8441</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
       <c r="A36">
         <v>5749</v>
       </c>
@@ -3615,8 +4384,22 @@
         <f t="shared" si="2"/>
         <v>7077.9972551835881</v>
       </c>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="O36" s="5">
+        <v>0.62909999999999999</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="3"/>
+        <v>62.91</v>
+      </c>
+      <c r="Q36">
+        <v>7078</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="4"/>
+        <v>4452.7698</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
       <c r="A37">
         <v>4298</v>
       </c>
@@ -3647,8 +4430,22 @@
         <f t="shared" si="2"/>
         <v>5660.9965166266884</v>
       </c>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="O37" s="5">
+        <v>0.59870000000000001</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="3"/>
+        <v>59.870000000000005</v>
+      </c>
+      <c r="Q37">
+        <v>5661</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="4"/>
+        <v>3389.2406999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
       <c r="A38">
         <v>926</v>
       </c>
@@ -3679,8 +4476,18 @@
         <f t="shared" si="2"/>
         <v>3056.9985322667599</v>
       </c>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="O38" s="5">
+        <v>0.19170000000000001</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="3"/>
+        <v>19.170000000000002</v>
+      </c>
+      <c r="Q38">
+        <v>3057</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
       <c r="A39">
         <v>1294</v>
       </c>
@@ -3711,8 +4518,22 @@
         <f t="shared" si="2"/>
         <v>1954.0010937490399</v>
       </c>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="O39" s="5">
+        <v>0.52659999999999996</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="3"/>
+        <v>52.66</v>
+      </c>
+      <c r="Q39">
+        <v>1954</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="4"/>
+        <v>1028.9764</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
       <c r="A40">
         <v>6579</v>
       </c>
@@ -3743,8 +4564,22 @@
         <f t="shared" si="2"/>
         <v>9247.0066570322524</v>
       </c>
-    </row>
-    <row r="41" spans="1:12">
+      <c r="O40" s="5">
+        <v>0.56040000000000001</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="3"/>
+        <v>56.04</v>
+      </c>
+      <c r="Q40">
+        <v>9247</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="4"/>
+        <v>5182.0187999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
       <c r="A41">
         <v>9784</v>
       </c>
@@ -3775,8 +4610,22 @@
         <f t="shared" si="2"/>
         <v>14237.989889028086</v>
       </c>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="O41" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="Q41">
+        <v>14238</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="4"/>
+        <v>7546.14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
       <c r="A42">
         <v>7315</v>
       </c>
@@ -3807,8 +4656,22 @@
         <f t="shared" si="2"/>
         <v>9858.9934655508423</v>
       </c>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="O42" s="5">
+        <v>0.56410000000000005</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="3"/>
+        <v>56.410000000000004</v>
+      </c>
+      <c r="Q42">
+        <v>9859</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="4"/>
+        <v>5561.4619000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
       <c r="A43">
         <v>2272</v>
       </c>
@@ -3839,8 +4702,22 @@
         <f t="shared" si="2"/>
         <v>5566.9979185218772</v>
       </c>
-    </row>
-    <row r="44" spans="1:12">
+      <c r="O43" s="5">
+        <v>0.21340000000000001</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="3"/>
+        <v>21.34</v>
+      </c>
+      <c r="Q43">
+        <v>5567</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="4"/>
+        <v>1187.9978000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
       <c r="A44">
         <v>15028</v>
       </c>
@@ -3871,8 +4748,22 @@
         <f t="shared" si="2"/>
         <v>19532.995305265107</v>
       </c>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="O44" s="5">
+        <v>0.59509999999999996</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="3"/>
+        <v>59.51</v>
+      </c>
+      <c r="Q44">
+        <v>19533</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="4"/>
+        <v>11624.088299999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
       <c r="A45">
         <v>6811</v>
       </c>
@@ -3903,8 +4794,22 @@
         <f t="shared" si="2"/>
         <v>8500.9958346550466</v>
       </c>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="O45" s="5">
+        <v>0.62019999999999997</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="3"/>
+        <v>62.019999999999996</v>
+      </c>
+      <c r="Q45">
+        <v>8501</v>
+      </c>
+      <c r="R45">
+        <f t="shared" si="4"/>
+        <v>5272.3202000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
       <c r="A46">
         <v>11948</v>
       </c>
@@ -3935,8 +4840,22 @@
         <f t="shared" si="2"/>
         <v>18363.014107166753</v>
       </c>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="O46" s="5">
+        <v>0.45590000000000003</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="3"/>
+        <v>45.59</v>
+      </c>
+      <c r="Q46">
+        <v>18363</v>
+      </c>
+      <c r="R46">
+        <f t="shared" si="4"/>
+        <v>8371.6917000000012</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
       <c r="A47">
         <v>8282</v>
       </c>
@@ -3967,8 +4886,22 @@
         <f t="shared" si="2"/>
         <v>9408.9977069096603</v>
       </c>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="O47" s="5">
+        <v>0.65149999999999997</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="3"/>
+        <v>65.149999999999991</v>
+      </c>
+      <c r="Q47">
+        <v>9409</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="4"/>
+        <v>6129.9634999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
       <c r="A48">
         <v>5407</v>
       </c>
@@ -3999,8 +4932,22 @@
         <f t="shared" si="2"/>
         <v>30836.048798200485</v>
       </c>
-    </row>
-    <row r="49" spans="1:12">
+      <c r="O48" s="5">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="3"/>
+        <v>7.2499999999999991</v>
+      </c>
+      <c r="Q48">
+        <v>30836</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="4"/>
+        <v>2235.6099999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18">
       <c r="A49">
         <v>6203</v>
       </c>
@@ -4031,8 +4978,22 @@
         <f t="shared" si="2"/>
         <v>7108.9989433725987</v>
       </c>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="O49" s="5">
+        <v>0.64580000000000004</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="3"/>
+        <v>64.58</v>
+      </c>
+      <c r="Q49">
+        <v>7109</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="4"/>
+        <v>4590.9922000000006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18">
       <c r="A50">
         <v>2416</v>
       </c>
@@ -4063,8 +5024,22 @@
         <f t="shared" si="2"/>
         <v>4190.9979803049227</v>
       </c>
-    </row>
-    <row r="51" spans="1:12">
+      <c r="O50" s="5">
+        <v>0.43759999999999999</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="3"/>
+        <v>43.76</v>
+      </c>
+      <c r="Q50">
+        <v>4191</v>
+      </c>
+      <c r="R50">
+        <f t="shared" si="4"/>
+        <v>1833.9815999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18">
       <c r="A51">
         <v>602</v>
       </c>
@@ -4095,8 +5070,22 @@
         <f t="shared" si="2"/>
         <v>3121.9930552650294</v>
       </c>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="O51" s="5">
+        <v>7.2099999999999997E-2</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="3"/>
+        <v>7.21</v>
+      </c>
+      <c r="Q51">
+        <v>3122</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="4"/>
+        <v>225.09619999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18">
       <c r="A52">
         <v>1727</v>
       </c>
@@ -4127,8 +5116,22 @@
         <f t="shared" si="2"/>
         <v>2764.0012052804313</v>
       </c>
-    </row>
-    <row r="53" spans="1:12">
+      <c r="O52" s="5">
+        <v>0.43890000000000001</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="3"/>
+        <v>43.89</v>
+      </c>
+      <c r="Q52">
+        <v>2764</v>
+      </c>
+      <c r="R52">
+        <f t="shared" si="4"/>
+        <v>1213.1196</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18">
       <c r="A53">
         <v>8707</v>
       </c>
@@ -4159,8 +5162,22 @@
         <f t="shared" si="2"/>
         <v>14512.001887073036</v>
       </c>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="O53" s="5">
+        <v>0.44919999999999999</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="3"/>
+        <v>44.92</v>
+      </c>
+      <c r="Q53">
+        <v>14512</v>
+      </c>
+      <c r="R53">
+        <f t="shared" si="4"/>
+        <v>6518.7903999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18">
       <c r="A54">
         <v>3054</v>
       </c>
@@ -4191,8 +5208,22 @@
         <f t="shared" si="2"/>
         <v>12353.994822084413</v>
       </c>
-    </row>
-    <row r="55" spans="1:12">
+      <c r="O54" s="5">
+        <v>0.15989999999999999</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="3"/>
+        <v>15.989999999999998</v>
+      </c>
+      <c r="Q54">
+        <v>12354</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="4"/>
+        <v>1975.4045999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18">
       <c r="A55">
         <v>533</v>
       </c>
@@ -4223,8 +5254,22 @@
         <f t="shared" si="2"/>
         <v>3167.9970183557475</v>
       </c>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="O55" s="5">
+        <v>8.5500000000000007E-2</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="3"/>
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="Q55">
+        <v>3168</v>
+      </c>
+      <c r="R55">
+        <f t="shared" si="4"/>
+        <v>270.86400000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18">
       <c r="A56">
         <v>1033</v>
       </c>
@@ -4255,8 +5300,22 @@
         <f t="shared" si="2"/>
         <v>4603.0011567542033</v>
       </c>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="O56" s="5">
+        <v>0.1101</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="3"/>
+        <v>11.01</v>
+      </c>
+      <c r="Q56">
+        <v>4603</v>
+      </c>
+      <c r="R56">
+        <f t="shared" si="4"/>
+        <v>506.7903</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18">
       <c r="A57">
         <v>2495</v>
       </c>
@@ -4287,8 +5346,22 @@
         <f t="shared" si="2"/>
         <v>6126.0001821309816</v>
       </c>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="O57" s="5">
+        <v>0.28239999999999998</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="3"/>
+        <v>28.24</v>
+      </c>
+      <c r="Q57">
+        <v>6126</v>
+      </c>
+      <c r="R57">
+        <f t="shared" si="4"/>
+        <v>1729.9823999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18">
       <c r="A58">
         <v>11323</v>
       </c>
@@ -4319,8 +5392,22 @@
         <f t="shared" si="2"/>
         <v>12495.004630438372</v>
       </c>
-    </row>
-    <row r="59" spans="1:12">
+      <c r="O58" s="5">
+        <v>0.65329999999999999</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="3"/>
+        <v>65.33</v>
+      </c>
+      <c r="Q58">
+        <v>12495</v>
+      </c>
+      <c r="R58">
+        <f t="shared" si="4"/>
+        <v>8162.9835000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18">
       <c r="A59">
         <v>15837</v>
       </c>
@@ -4351,8 +5438,22 @@
         <f t="shared" si="2"/>
         <v>161382.39084523672</v>
       </c>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="O59" s="5">
+        <v>1.01E-2</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="3"/>
+        <v>1.01</v>
+      </c>
+      <c r="Q59">
+        <v>161382</v>
+      </c>
+      <c r="R59">
+        <f t="shared" si="4"/>
+        <v>1629.9582</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18">
       <c r="A60">
         <v>1256</v>
       </c>
@@ -4383,8 +5484,22 @@
         <f t="shared" si="2"/>
         <v>2121.9986799492499</v>
       </c>
-    </row>
-    <row r="61" spans="1:12">
+      <c r="O60" s="5">
+        <v>0.42270000000000002</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="3"/>
+        <v>42.27</v>
+      </c>
+      <c r="Q60">
+        <v>2122</v>
+      </c>
+      <c r="R60">
+        <f t="shared" si="4"/>
+        <v>896.96940000000006</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18">
       <c r="A61">
         <v>5094</v>
       </c>
@@ -4415,8 +5530,22 @@
         <f t="shared" si="2"/>
         <v>7600.0042653862383</v>
       </c>
-    </row>
-    <row r="62" spans="1:12">
+      <c r="O61" s="5">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="3"/>
+        <v>52.2</v>
+      </c>
+      <c r="Q61">
+        <v>7600</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="4"/>
+        <v>3967.2000000000003</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18">
       <c r="A62">
         <v>2751</v>
       </c>
@@ -4447,8 +5576,22 @@
         <f t="shared" si="2"/>
         <v>8666.0085148392682</v>
       </c>
-    </row>
-    <row r="63" spans="1:12">
+      <c r="O62" s="5">
+        <v>0.18149999999999999</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="3"/>
+        <v>18.149999999999999</v>
+      </c>
+      <c r="Q62">
+        <v>8666</v>
+      </c>
+      <c r="R62">
+        <f t="shared" si="4"/>
+        <v>1572.8789999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18">
       <c r="A63">
         <v>7789</v>
       </c>
@@ -4479,8 +5622,22 @@
         <f t="shared" si="2"/>
         <v>11133.005502183916</v>
       </c>
-    </row>
-    <row r="64" spans="1:12">
+      <c r="O63" s="5">
+        <v>0.52729999999999999</v>
+      </c>
+      <c r="P63">
+        <f t="shared" si="3"/>
+        <v>52.73</v>
+      </c>
+      <c r="Q63">
+        <v>11133</v>
+      </c>
+      <c r="R63">
+        <f t="shared" si="4"/>
+        <v>5870.4309000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18">
       <c r="A64">
         <v>595</v>
       </c>
@@ -4511,8 +5668,22 @@
         <f t="shared" si="2"/>
         <v>6614.9999113270787</v>
       </c>
-    </row>
-    <row r="65" spans="1:12">
+      <c r="O64" s="5">
+        <v>2.07E-2</v>
+      </c>
+      <c r="P64">
+        <f t="shared" si="3"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="Q64">
+        <v>6615</v>
+      </c>
+      <c r="R64">
+        <f t="shared" si="4"/>
+        <v>136.93049999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18">
       <c r="A65">
         <v>11841</v>
       </c>
@@ -4543,8 +5714,22 @@
         <f t="shared" si="2"/>
         <v>43388.997972536505</v>
       </c>
-    </row>
-    <row r="66" spans="1:12">
+      <c r="O65" s="5">
+        <v>0.154</v>
+      </c>
+      <c r="P65">
+        <f t="shared" si="3"/>
+        <v>15.4</v>
+      </c>
+      <c r="Q65">
+        <v>43389</v>
+      </c>
+      <c r="R65">
+        <f t="shared" si="4"/>
+        <v>6681.9059999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18">
       <c r="A66">
         <v>99</v>
       </c>
@@ -4575,8 +5760,22 @@
         <f t="shared" si="2"/>
         <v>533.99956135750313</v>
       </c>
-    </row>
-    <row r="67" spans="1:12">
+      <c r="O66" s="5">
+        <v>0.1236</v>
+      </c>
+      <c r="P66">
+        <f t="shared" si="3"/>
+        <v>12.36</v>
+      </c>
+      <c r="Q66">
+        <v>534</v>
+      </c>
+      <c r="R66">
+        <f t="shared" si="4"/>
+        <v>66.002399999999994</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18">
       <c r="A67">
         <v>208</v>
       </c>
@@ -4584,7 +5783,7 @@
         <v>42.1907</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:C97" si="3">100/B67 * A67</f>
+        <f t="shared" ref="C67:C97" si="5">100/B67 * A67</f>
         <v>492.99964210122135</v>
       </c>
       <c r="E67">
@@ -4594,7 +5793,7 @@
         <v>0.25</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G97" si="4">1/F67*E67</f>
+        <f t="shared" ref="G67:G97" si="6">1/F67*E67</f>
         <v>480</v>
       </c>
       <c r="J67">
@@ -4604,11 +5803,25 @@
         <v>0.43333300000000002</v>
       </c>
       <c r="L67">
-        <f t="shared" ref="L67:L97" si="5">J67*1/K67</f>
+        <f t="shared" ref="L67:L97" si="7">J67*1/K67</f>
         <v>480.00036923105324</v>
       </c>
-    </row>
-    <row r="68" spans="1:12">
+      <c r="O67" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="P67">
+        <f t="shared" ref="P67:P97" si="8">O67*100</f>
+        <v>30</v>
+      </c>
+      <c r="Q67">
+        <v>480</v>
+      </c>
+      <c r="R67">
+        <f t="shared" ref="R67:R97" si="9">Q67*O67</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18">
       <c r="A68">
         <v>1443</v>
       </c>
@@ -4616,7 +5829,7 @@
         <v>85.384600000000006</v>
       </c>
       <c r="C68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1690.0003045045594</v>
       </c>
       <c r="E68">
@@ -4626,7 +5839,7 @@
         <v>0.59</v>
       </c>
       <c r="G68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1638.9830508474577</v>
       </c>
       <c r="J68">
@@ -4636,11 +5849,25 @@
         <v>0.85103799999999996</v>
       </c>
       <c r="L68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1637.9997132912986</v>
       </c>
-    </row>
-    <row r="69" spans="1:12">
+      <c r="O68" s="5">
+        <v>0.70389999999999997</v>
+      </c>
+      <c r="P68">
+        <f t="shared" si="8"/>
+        <v>70.39</v>
+      </c>
+      <c r="Q68">
+        <v>1638</v>
+      </c>
+      <c r="R68">
+        <f t="shared" si="9"/>
+        <v>1152.9882</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18">
       <c r="A69">
         <v>4057</v>
       </c>
@@ -4648,7 +5875,7 @@
         <v>60.488999999999997</v>
       </c>
       <c r="C69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6707.0045793450054</v>
       </c>
       <c r="E69">
@@ -4658,7 +5885,7 @@
         <v>0.35799999999999998</v>
       </c>
       <c r="G69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6569.8324022346369</v>
       </c>
       <c r="J69">
@@ -4668,11 +5895,25 @@
         <v>0.61444699999999997</v>
       </c>
       <c r="L69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6561.9980242396823</v>
       </c>
-    </row>
-    <row r="70" spans="1:12">
+      <c r="O69" s="5">
+        <v>0.4526</v>
+      </c>
+      <c r="P69">
+        <f t="shared" si="8"/>
+        <v>45.26</v>
+      </c>
+      <c r="Q69">
+        <v>6562</v>
+      </c>
+      <c r="R69">
+        <f t="shared" si="9"/>
+        <v>2969.9612000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18">
       <c r="A70">
         <v>476</v>
       </c>
@@ -4680,7 +5921,7 @@
         <v>62.879800000000003</v>
       </c>
       <c r="C70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>756.99986323111705</v>
       </c>
       <c r="E70">
@@ -4690,7 +5931,7 @@
         <v>0.33700000000000002</v>
       </c>
       <c r="G70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>732.93768545994067</v>
       </c>
       <c r="J70">
@@ -4700,11 +5941,25 @@
         <v>0.61885199999999996</v>
       </c>
       <c r="L70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>732.00054294080007</v>
       </c>
-    </row>
-    <row r="71" spans="1:12">
+      <c r="O70" s="5">
+        <v>0.44669999999999999</v>
+      </c>
+      <c r="P70">
+        <f t="shared" si="8"/>
+        <v>44.67</v>
+      </c>
+      <c r="Q70">
+        <v>732</v>
+      </c>
+      <c r="R70">
+        <f t="shared" si="9"/>
+        <v>326.98439999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18">
       <c r="A71">
         <v>195</v>
       </c>
@@ -4712,7 +5967,7 @@
         <v>42.951500000000003</v>
       </c>
       <c r="C71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>454.00044235940533</v>
       </c>
       <c r="E71">
@@ -4722,7 +5977,7 @@
         <v>0.22</v>
       </c>
       <c r="G71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>450.00000000000006</v>
       </c>
       <c r="J71">
@@ -4732,11 +5987,25 @@
         <v>0.45898</v>
       </c>
       <c r="L71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>451.00004357488342</v>
       </c>
-    </row>
-    <row r="72" spans="1:12">
+      <c r="O71" s="5">
+        <v>0.2949</v>
+      </c>
+      <c r="P71">
+        <f t="shared" si="8"/>
+        <v>29.49</v>
+      </c>
+      <c r="Q71">
+        <v>451</v>
+      </c>
+      <c r="R71">
+        <f t="shared" si="9"/>
+        <v>132.9999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18">
       <c r="A72">
         <v>219</v>
       </c>
@@ -4744,7 +6013,7 @@
         <v>57.180199999999999</v>
       </c>
       <c r="C72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>382.9997096897178</v>
       </c>
       <c r="E72">
@@ -4754,7 +6023,7 @@
         <v>0.38400000000000001</v>
       </c>
       <c r="G72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>372.39583333333331</v>
       </c>
       <c r="J72">
@@ -4764,11 +6033,25 @@
         <v>0.55645199999999995</v>
       </c>
       <c r="L72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>371.99974121757134</v>
       </c>
-    </row>
-    <row r="73" spans="1:12">
+      <c r="O72" s="5">
+        <v>0.44090000000000001</v>
+      </c>
+      <c r="P72">
+        <f t="shared" si="8"/>
+        <v>44.09</v>
+      </c>
+      <c r="Q72">
+        <v>372</v>
+      </c>
+      <c r="R72">
+        <f t="shared" si="9"/>
+        <v>164.01480000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18">
       <c r="A73">
         <v>1035</v>
       </c>
@@ -4776,7 +6059,7 @@
         <v>38.037500000000001</v>
       </c>
       <c r="C73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2720.9990141307917</v>
       </c>
       <c r="E73">
@@ -4786,7 +6069,7 @@
         <v>0.16</v>
       </c>
       <c r="G73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2693.75</v>
       </c>
       <c r="J73">
@@ -4796,11 +6079,25 @@
         <v>0.394345</v>
       </c>
       <c r="L73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2688.0016229443763</v>
       </c>
-    </row>
-    <row r="74" spans="1:12">
+      <c r="O73" s="5">
+        <v>0.224</v>
+      </c>
+      <c r="P73">
+        <f t="shared" si="8"/>
+        <v>22.400000000000002</v>
+      </c>
+      <c r="Q73">
+        <v>2688</v>
+      </c>
+      <c r="R73">
+        <f t="shared" si="9"/>
+        <v>602.11199999999997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18">
       <c r="A74">
         <v>7723</v>
       </c>
@@ -4808,7 +6105,7 @@
         <v>70.710499999999996</v>
       </c>
       <c r="C74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10921.998854484131</v>
       </c>
       <c r="E74">
@@ -4818,7 +6115,7 @@
         <v>0.438</v>
       </c>
       <c r="G74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10657.534246575344</v>
       </c>
       <c r="J74">
@@ -4828,11 +6125,25 @@
         <v>0.70129600000000003</v>
       </c>
       <c r="L74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>10646.003969793068</v>
       </c>
-    </row>
-    <row r="75" spans="1:12">
+      <c r="O74" s="5">
+        <v>0.55630000000000002</v>
+      </c>
+      <c r="P74">
+        <f t="shared" si="8"/>
+        <v>55.63</v>
+      </c>
+      <c r="Q74">
+        <v>10646</v>
+      </c>
+      <c r="R74">
+        <f t="shared" si="9"/>
+        <v>5922.3698000000004</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18">
       <c r="A75">
         <v>3534</v>
       </c>
@@ -4840,7 +6151,7 @@
         <v>72.805899999999994</v>
       </c>
       <c r="C75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4854.0022168533051</v>
       </c>
       <c r="E75">
@@ -4850,7 +6161,7 @@
         <v>0.47799999999999998</v>
       </c>
       <c r="G75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4721.757322175732</v>
       </c>
       <c r="J75">
@@ -4860,11 +6171,25 @@
         <v>0.72779300000000002</v>
       </c>
       <c r="L75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4717.0005757131494</v>
       </c>
-    </row>
-    <row r="76" spans="1:12">
+      <c r="O75" s="5">
+        <v>0.59589999999999999</v>
+      </c>
+      <c r="P75">
+        <f t="shared" si="8"/>
+        <v>59.589999999999996</v>
+      </c>
+      <c r="Q75">
+        <v>4717</v>
+      </c>
+      <c r="R75">
+        <f t="shared" si="9"/>
+        <v>2810.8602999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18">
       <c r="A76">
         <v>1322</v>
       </c>
@@ -4872,7 +6197,7 @@
         <v>70.207099999999997</v>
       </c>
       <c r="C76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1883.0004372777114</v>
       </c>
       <c r="E76">
@@ -4882,7 +6207,7 @@
         <v>0.39500000000000002</v>
       </c>
       <c r="G76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1820.2531645569618</v>
       </c>
       <c r="J76">
@@ -4892,11 +6217,25 @@
         <v>0.70950000000000002</v>
       </c>
       <c r="L76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1821.000704721635</v>
       </c>
-    </row>
-    <row r="77" spans="1:12">
+      <c r="O76" s="5">
+        <v>0.52549999999999997</v>
+      </c>
+      <c r="P76">
+        <f t="shared" si="8"/>
+        <v>52.55</v>
+      </c>
+      <c r="Q76">
+        <v>1821</v>
+      </c>
+      <c r="R76">
+        <f t="shared" si="9"/>
+        <v>956.93549999999993</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18">
       <c r="A77">
         <v>9914</v>
       </c>
@@ -4904,7 +6243,7 @@
         <v>41.399799999999999</v>
       </c>
       <c r="C77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>23946.975589254052</v>
       </c>
       <c r="E77">
@@ -4914,7 +6253,7 @@
         <v>0.20300000000000001</v>
       </c>
       <c r="G77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>23610.837438423641</v>
       </c>
       <c r="J77">
@@ -4924,11 +6263,25 @@
         <v>0.43541099999999999</v>
       </c>
       <c r="L77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>23602.986603462017</v>
       </c>
-    </row>
-    <row r="78" spans="1:12">
+      <c r="O77" s="5">
+        <v>0.27679999999999999</v>
+      </c>
+      <c r="P77">
+        <f t="shared" si="8"/>
+        <v>27.68</v>
+      </c>
+      <c r="Q77">
+        <v>23603</v>
+      </c>
+      <c r="R77">
+        <f t="shared" si="9"/>
+        <v>6533.3103999999994</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18">
       <c r="A78">
         <v>233</v>
       </c>
@@ -4936,7 +6289,7 @@
         <v>64.010999999999996</v>
       </c>
       <c r="C78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>363.99993751074032</v>
       </c>
       <c r="E78">
@@ -4946,7 +6299,7 @@
         <v>0.36099999999999999</v>
       </c>
       <c r="G78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>354.5706371191136</v>
       </c>
       <c r="J78">
@@ -4956,11 +6309,25 @@
         <v>0.61690100000000003</v>
       </c>
       <c r="L78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>355.0002350458177</v>
       </c>
-    </row>
-    <row r="79" spans="1:12">
+      <c r="O78" s="5">
+        <v>0.4451</v>
+      </c>
+      <c r="P78">
+        <f t="shared" si="8"/>
+        <v>44.51</v>
+      </c>
+      <c r="Q78">
+        <v>355</v>
+      </c>
+      <c r="R78">
+        <f t="shared" si="9"/>
+        <v>158.01050000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18">
       <c r="A79">
         <v>1457</v>
       </c>
@@ -4968,7 +6335,7 @@
         <v>70.183000000000007</v>
       </c>
       <c r="C79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2076.001310858755</v>
       </c>
       <c r="E79">
@@ -4978,7 +6345,7 @@
         <v>0.379</v>
       </c>
       <c r="G79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2055.4089709762534</v>
       </c>
       <c r="J79">
@@ -4988,11 +6355,25 @@
         <v>0.71123000000000003</v>
       </c>
       <c r="L79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2056.9998453383573</v>
       </c>
-    </row>
-    <row r="80" spans="1:12">
+      <c r="O79" s="5">
+        <v>0.51819999999999999</v>
+      </c>
+      <c r="P79">
+        <f t="shared" si="8"/>
+        <v>51.82</v>
+      </c>
+      <c r="Q79">
+        <v>2057</v>
+      </c>
+      <c r="R79">
+        <f t="shared" si="9"/>
+        <v>1065.9374</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18">
       <c r="A80">
         <v>5671</v>
       </c>
@@ -5000,7 +6381,7 @@
         <v>91.808300000000003</v>
       </c>
       <c r="C80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6177.0014257970142</v>
       </c>
       <c r="E80">
@@ -5010,7 +6391,7 @@
         <v>0.59699999999999998</v>
       </c>
       <c r="G80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5765.4941373534339</v>
       </c>
       <c r="J80">
@@ -5020,11 +6401,25 @@
         <v>0.909501</v>
       </c>
       <c r="L80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5767.9980560769036</v>
       </c>
-    </row>
-    <row r="81" spans="1:12">
+      <c r="O80" s="5">
+        <v>0.73939999999999995</v>
+      </c>
+      <c r="P80">
+        <f t="shared" si="8"/>
+        <v>73.94</v>
+      </c>
+      <c r="Q80">
+        <v>5768</v>
+      </c>
+      <c r="R80">
+        <f t="shared" si="9"/>
+        <v>4264.8591999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18">
       <c r="A81">
         <v>4282</v>
       </c>
@@ -5032,7 +6427,7 @@
         <v>58.729900000000001</v>
       </c>
       <c r="C81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7291.0050928062201</v>
       </c>
       <c r="E81">
@@ -5042,7 +6437,7 @@
         <v>0.36099999999999999</v>
       </c>
       <c r="G81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7063.7119113573408</v>
       </c>
       <c r="J81">
@@ -5052,11 +6447,25 @@
         <v>0.58569000000000004</v>
       </c>
       <c r="L81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7072.0005463641173</v>
       </c>
-    </row>
-    <row r="82" spans="1:12">
+      <c r="O81" s="5">
+        <v>0.45079999999999998</v>
+      </c>
+      <c r="P81">
+        <f t="shared" si="8"/>
+        <v>45.08</v>
+      </c>
+      <c r="Q81">
+        <v>7072</v>
+      </c>
+      <c r="R81">
+        <f t="shared" si="9"/>
+        <v>3188.0575999999996</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18">
       <c r="A82">
         <v>116</v>
       </c>
@@ -5064,7 +6473,7 @@
         <v>46.7742</v>
       </c>
       <c r="C82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>247.99996579310817</v>
       </c>
       <c r="E82">
@@ -5074,7 +6483,7 @@
         <v>0.214</v>
       </c>
       <c r="G82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>242.99065420560748</v>
       </c>
       <c r="J82">
@@ -5084,11 +6493,25 @@
         <v>0.48148099999999999</v>
       </c>
       <c r="L82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>243.00024300024302</v>
       </c>
-    </row>
-    <row r="83" spans="1:12">
+      <c r="O82" s="5">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="P82">
+        <f t="shared" si="8"/>
+        <v>33.33</v>
+      </c>
+      <c r="Q82">
+        <v>243</v>
+      </c>
+      <c r="R82">
+        <f t="shared" si="9"/>
+        <v>80.991900000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18">
       <c r="A83">
         <v>4578</v>
       </c>
@@ -5096,7 +6519,7 @@
         <v>44.637300000000003</v>
       </c>
       <c r="C83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10255.996666465042</v>
       </c>
       <c r="E83">
@@ -5106,7 +6529,7 @@
         <v>0.23699999999999999</v>
       </c>
       <c r="G83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10021.097046413503</v>
       </c>
       <c r="J83">
@@ -5116,11 +6539,25 @@
         <v>0.45794200000000002</v>
       </c>
       <c r="L83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>10010.001266535937</v>
       </c>
-    </row>
-    <row r="84" spans="1:12">
+      <c r="O83" s="5">
+        <v>0.30819999999999997</v>
+      </c>
+      <c r="P83">
+        <f t="shared" si="8"/>
+        <v>30.819999999999997</v>
+      </c>
+      <c r="Q83">
+        <v>10010</v>
+      </c>
+      <c r="R83">
+        <f t="shared" si="9"/>
+        <v>3085.0819999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18">
       <c r="A84">
         <v>2681</v>
       </c>
@@ -5128,7 +6565,7 @@
         <v>48.210799999999999</v>
       </c>
       <c r="C84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5560.9946319082028</v>
       </c>
       <c r="E84">
@@ -5138,7 +6575,7 @@
         <v>0.24199999999999999</v>
       </c>
       <c r="G84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5475.2066115702482</v>
       </c>
       <c r="J84">
@@ -5148,11 +6585,25 @@
         <v>0.49524699999999999</v>
       </c>
       <c r="L84">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5469.9977990780362</v>
       </c>
-    </row>
-    <row r="85" spans="1:12">
+      <c r="O84" s="5">
+        <v>0.34150000000000003</v>
+      </c>
+      <c r="P84">
+        <f t="shared" si="8"/>
+        <v>34.150000000000006</v>
+      </c>
+      <c r="Q84">
+        <v>5470</v>
+      </c>
+      <c r="R84">
+        <f t="shared" si="9"/>
+        <v>1868.0050000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18">
       <c r="A85">
         <v>928</v>
       </c>
@@ -5160,7 +6611,7 @@
         <v>17.0213</v>
       </c>
       <c r="C85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5451.9925035103079</v>
       </c>
       <c r="E85">
@@ -5170,7 +6621,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="G85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5390.8045977011498</v>
       </c>
       <c r="J85">
@@ -5180,11 +6631,25 @@
         <v>0.173066</v>
       </c>
       <c r="L85">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5391.0068991020771</v>
       </c>
-    </row>
-    <row r="86" spans="1:12">
+      <c r="O85" s="5">
+        <v>0.105</v>
+      </c>
+      <c r="P85">
+        <f t="shared" si="8"/>
+        <v>10.5</v>
+      </c>
+      <c r="Q85">
+        <v>5391</v>
+      </c>
+      <c r="R85">
+        <f t="shared" si="9"/>
+        <v>566.05499999999995</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18">
       <c r="A86">
         <v>2141</v>
       </c>
@@ -5192,7 +6657,7 @@
         <v>46.9724</v>
       </c>
       <c r="C86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4557.9957592117926</v>
       </c>
       <c r="E86">
@@ -5202,7 +6667,7 @@
         <v>0.219</v>
       </c>
       <c r="G86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4447.488584474886</v>
       </c>
       <c r="J86">
@@ -5212,11 +6677,25 @@
         <v>0.47206599999999999</v>
       </c>
       <c r="L86">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4457.0038935233633</v>
       </c>
-    </row>
-    <row r="87" spans="1:12">
+      <c r="O86" s="5">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="P86">
+        <f t="shared" si="8"/>
+        <v>30.2</v>
+      </c>
+      <c r="Q86">
+        <v>4457</v>
+      </c>
+      <c r="R86">
+        <f t="shared" si="9"/>
+        <v>1346.0139999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18">
       <c r="A87">
         <v>3030</v>
       </c>
@@ -5224,7 +6703,7 @@
         <v>54.398600000000002</v>
       </c>
       <c r="C87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5569.9962866691421</v>
       </c>
       <c r="E87">
@@ -5234,7 +6713,7 @@
         <v>0.311</v>
       </c>
       <c r="G87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5395.4983922829579</v>
       </c>
       <c r="J87">
@@ -5244,11 +6723,25 @@
         <v>0.56125100000000006</v>
       </c>
       <c r="L87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5403.999280179456</v>
       </c>
-    </row>
-    <row r="88" spans="1:12">
+      <c r="O87" s="5">
+        <v>0.39119999999999999</v>
+      </c>
+      <c r="P87">
+        <f t="shared" si="8"/>
+        <v>39.119999999999997</v>
+      </c>
+      <c r="Q87">
+        <v>5404</v>
+      </c>
+      <c r="R87">
+        <f t="shared" si="9"/>
+        <v>2114.0448000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18">
       <c r="A88">
         <v>984</v>
       </c>
@@ -5256,7 +6749,7 @@
         <v>17.290500000000002</v>
       </c>
       <c r="C88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5690.9863798039387</v>
       </c>
       <c r="E88">
@@ -5266,7 +6759,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="G88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5606.060606060606</v>
       </c>
       <c r="J88">
@@ -5276,11 +6769,25 @@
         <v>0.18664500000000001</v>
       </c>
       <c r="L88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5631.0107423183044</v>
       </c>
-    </row>
-    <row r="89" spans="1:12">
+      <c r="O88" s="5">
+        <v>9.9400000000000002E-2</v>
+      </c>
+      <c r="P88">
+        <f t="shared" si="8"/>
+        <v>9.94</v>
+      </c>
+      <c r="Q88">
+        <v>5631</v>
+      </c>
+      <c r="R88">
+        <f t="shared" si="9"/>
+        <v>559.72140000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18">
       <c r="A89">
         <v>3175</v>
       </c>
@@ -5288,7 +6795,7 @@
         <v>43.445500000000003</v>
       </c>
       <c r="C89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7308.0065829602599</v>
       </c>
       <c r="E89">
@@ -5298,7 +6805,7 @@
         <v>0.255</v>
       </c>
       <c r="G89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7196.0784313725489</v>
       </c>
       <c r="J89">
@@ -5308,11 +6815,25 @@
         <v>0.44814100000000001</v>
       </c>
       <c r="L89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7183.007133915442</v>
       </c>
-    </row>
-    <row r="90" spans="1:12">
+      <c r="O89" s="5">
+        <v>0.31309999999999999</v>
+      </c>
+      <c r="P89">
+        <f t="shared" si="8"/>
+        <v>31.31</v>
+      </c>
+      <c r="Q89">
+        <v>7183</v>
+      </c>
+      <c r="R89">
+        <f t="shared" si="9"/>
+        <v>2248.9973</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18">
       <c r="A90">
         <v>7716</v>
       </c>
@@ -5320,7 +6841,7 @@
         <v>51.532800000000002</v>
       </c>
       <c r="C90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14972.988077496273</v>
       </c>
       <c r="E90">
@@ -5330,7 +6851,7 @@
         <v>0.35799999999999998</v>
       </c>
       <c r="G90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>14695.530726256982</v>
       </c>
       <c r="J90">
@@ -5340,11 +6861,25 @@
         <v>0.51166599999999995</v>
       </c>
       <c r="L90">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>14700.996353089713</v>
       </c>
-    </row>
-    <row r="91" spans="1:12">
+      <c r="O90" s="5">
+        <v>0.4138</v>
+      </c>
+      <c r="P90">
+        <f t="shared" si="8"/>
+        <v>41.38</v>
+      </c>
+      <c r="Q90">
+        <v>14701</v>
+      </c>
+      <c r="R90">
+        <f t="shared" si="9"/>
+        <v>6083.2737999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18">
       <c r="A91">
         <v>7725</v>
       </c>
@@ -5352,7 +6887,7 @@
         <v>57.865200000000002</v>
       </c>
       <c r="C91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>13349.992741751517</v>
       </c>
       <c r="E91">
@@ -5362,7 +6897,7 @@
         <v>0.30299999999999999</v>
       </c>
       <c r="G91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>13135.313531353135</v>
       </c>
       <c r="J91">
@@ -5372,11 +6907,25 @@
         <v>0.58241299999999996</v>
       </c>
       <c r="L91">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>13135.009005636894</v>
       </c>
-    </row>
-    <row r="92" spans="1:12">
+      <c r="O91" s="5">
+        <v>0.39939999999999998</v>
+      </c>
+      <c r="P91">
+        <f t="shared" si="8"/>
+        <v>39.94</v>
+      </c>
+      <c r="Q91">
+        <v>13135</v>
+      </c>
+      <c r="R91">
+        <f t="shared" si="9"/>
+        <v>5246.1189999999997</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18">
       <c r="A92">
         <v>4615</v>
       </c>
@@ -5384,7 +6933,7 @@
         <v>39.206499999999998</v>
       </c>
       <c r="C92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11771.007358473722</v>
       </c>
       <c r="E92">
@@ -5394,7 +6943,7 @@
         <v>0.123</v>
       </c>
       <c r="G92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>11731.707317073171</v>
       </c>
       <c r="J92">
@@ -5404,11 +6953,25 @@
         <v>0.41842600000000002</v>
       </c>
       <c r="L92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>11700.993724099362</v>
       </c>
-    </row>
-    <row r="93" spans="1:12">
+      <c r="O92" s="5">
+        <v>0.1961</v>
+      </c>
+      <c r="P92">
+        <f t="shared" si="8"/>
+        <v>19.61</v>
+      </c>
+      <c r="Q92">
+        <v>11701</v>
+      </c>
+      <c r="R92">
+        <f t="shared" si="9"/>
+        <v>2294.5661</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18">
       <c r="A93">
         <v>4785</v>
       </c>
@@ -5416,7 +6979,7 @@
         <v>29.681799999999999</v>
       </c>
       <c r="C93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>16120.989966915755</v>
       </c>
       <c r="E93">
@@ -5426,7 +6989,7 @@
         <v>0.159</v>
       </c>
       <c r="G93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>15911.94968553459</v>
       </c>
       <c r="J93">
@@ -5436,11 +6999,25 @@
         <v>0.29883999999999999</v>
       </c>
       <c r="L93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>15955.026100923571</v>
       </c>
-    </row>
-    <row r="94" spans="1:12">
+      <c r="O93" s="5">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="P93">
+        <f t="shared" si="8"/>
+        <v>20.599999999999998</v>
+      </c>
+      <c r="Q93">
+        <v>15955</v>
+      </c>
+      <c r="R93">
+        <f t="shared" si="9"/>
+        <v>3286.73</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18">
       <c r="A94">
         <v>1728</v>
       </c>
@@ -5448,7 +7025,7 @@
         <v>21.1066</v>
       </c>
       <c r="C94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8187.0125932172878</v>
       </c>
       <c r="E94">
@@ -5458,7 +7035,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="G94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8125.0000000000009</v>
       </c>
       <c r="J94">
@@ -5468,11 +7045,25 @@
         <v>0.24455099999999999</v>
       </c>
       <c r="L94">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8121.0054344492564</v>
       </c>
-    </row>
-    <row r="95" spans="1:12">
+      <c r="O94" s="5">
+        <v>0.1196</v>
+      </c>
+      <c r="P94">
+        <f t="shared" si="8"/>
+        <v>11.959999999999999</v>
+      </c>
+      <c r="Q94">
+        <v>8121</v>
+      </c>
+      <c r="R94">
+        <f t="shared" si="9"/>
+        <v>971.27160000000003</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18">
       <c r="A95">
         <v>8475</v>
       </c>
@@ -5480,7 +7071,7 @@
         <v>82.828400000000002</v>
       </c>
       <c r="C95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10231.99772058859</v>
       </c>
       <c r="E95">
@@ -5490,7 +7081,7 @@
         <v>0.495</v>
       </c>
       <c r="G95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9949.4949494949506</v>
       </c>
       <c r="J95">
@@ -5500,11 +7091,25 @@
         <v>0.826376</v>
       </c>
       <c r="L95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9940.9953822473071</v>
       </c>
-    </row>
-    <row r="96" spans="1:12">
+      <c r="O95" s="5">
+        <v>0.65639999999999998</v>
+      </c>
+      <c r="P95">
+        <f t="shared" si="8"/>
+        <v>65.64</v>
+      </c>
+      <c r="Q95">
+        <v>9941</v>
+      </c>
+      <c r="R95">
+        <f t="shared" si="9"/>
+        <v>6525.2723999999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18">
       <c r="A96">
         <v>2630</v>
       </c>
@@ -5512,7 +7117,7 @@
         <v>62.768500000000003</v>
       </c>
       <c r="C96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4189.99976102663</v>
       </c>
       <c r="E96">
@@ -5522,7 +7127,7 @@
         <v>0.35099999999999998</v>
       </c>
       <c r="G96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4079.7720797720804</v>
       </c>
       <c r="J96">
@@ -5532,11 +7137,25 @@
         <v>0.631992</v>
       </c>
       <c r="L96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4076.000962037494</v>
       </c>
-    </row>
-    <row r="97" spans="1:13">
+      <c r="O96" s="5">
+        <v>0.4526</v>
+      </c>
+      <c r="P96">
+        <f t="shared" si="8"/>
+        <v>45.26</v>
+      </c>
+      <c r="Q96">
+        <v>4076</v>
+      </c>
+      <c r="R96">
+        <f t="shared" si="9"/>
+        <v>1844.7976000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19">
       <c r="A97">
         <v>2166</v>
       </c>
@@ -5544,7 +7163,7 @@
         <v>57.407899999999998</v>
       </c>
       <c r="C97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3772.9998832913243</v>
       </c>
       <c r="E97">
@@ -5554,7 +7173,7 @@
         <v>0.30299999999999999</v>
       </c>
       <c r="G97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3686.4686468646864</v>
       </c>
       <c r="J97">
@@ -5564,11 +7183,25 @@
         <v>0.575183</v>
       </c>
       <c r="L97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3690.9992124245673</v>
       </c>
-    </row>
-    <row r="98" spans="1:13">
+      <c r="O97" s="5">
+        <v>0.41210000000000002</v>
+      </c>
+      <c r="P97">
+        <f t="shared" si="8"/>
+        <v>41.21</v>
+      </c>
+      <c r="Q97">
+        <v>3691</v>
+      </c>
+      <c r="R97">
+        <f t="shared" si="9"/>
+        <v>1521.0611000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19">
       <c r="A98">
         <f>SUM(A2:A97)</f>
         <v>384307</v>
@@ -5604,6 +7237,19 @@
       <c r="M98">
         <f>J98/L98</f>
         <v>0.46456942516291594</v>
+      </c>
+      <c r="O98" s="5"/>
+      <c r="Q98">
+        <f>SUM(Q2:Q97)</f>
+        <v>835683</v>
+      </c>
+      <c r="R98">
+        <f>SUM(R2:R97)</f>
+        <v>267283.68739999994</v>
+      </c>
+      <c r="S98">
+        <f>R98/Q98</f>
+        <v>0.31983860794104935</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added version numbers for the alignment tools and updated preprocessing.txt
</commit_message>
<xml_diff>
--- a/ComparingMappingRates.xlsx
+++ b/ComparingMappingRates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="1420" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="9200" yWindow="2380" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Comparisons" sheetId="2" r:id="rId1"/>
@@ -38,19 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t>BWA</t>
-  </si>
-  <si>
     <t>Cell ID</t>
-  </si>
-  <si>
-    <t>Tophat2</t>
-  </si>
-  <si>
-    <t>Bowtie2</t>
-  </si>
-  <si>
-    <t>**STAR**</t>
   </si>
   <si>
     <t>greater than 50%</t>
@@ -86,7 +74,19 @@
     <t>Overall Mapping Rate</t>
   </si>
   <si>
-    <t>HiSat2</t>
+    <t>BWA 0.7.15</t>
+  </si>
+  <si>
+    <t>Tophat2 v2.0.14</t>
+  </si>
+  <si>
+    <t>Bowtie2 version 2.3.2</t>
+  </si>
+  <si>
+    <t>HiSat2 2.1.0</t>
+  </si>
+  <si>
+    <t>**STAR** 2.5.3a</t>
   </si>
 </sst>
 </file>
@@ -99,7 +99,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -674,51 +673,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="24" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="B2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="B3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
         <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2545,7 +2542,7 @@
     </row>
     <row r="105" spans="1:8">
       <c r="A105" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B105">
         <f>COUNTIF(B6:B101, "&gt;=25")</f>
@@ -2566,7 +2563,7 @@
     </row>
     <row r="106" spans="1:8">
       <c r="A106" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B106">
         <f>COUNTIF(B6:B101, "&gt;=50")</f>
@@ -2587,7 +2584,7 @@
     </row>
     <row r="107" spans="1:8">
       <c r="A107" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B107">
         <f>COUNTIF(B6:B101, "&gt;=75")</f>
@@ -2608,7 +2605,7 @@
     </row>
     <row r="108" spans="1:8">
       <c r="A108" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B108">
         <f>COUNTIF(B7:B102, "&gt;=80")</f>
@@ -2629,7 +2626,7 @@
     </row>
     <row r="109" spans="1:8">
       <c r="A109" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B109">
         <f>COUNTIF(B6:B101, "&gt;=90")</f>
@@ -2650,7 +2647,7 @@
     </row>
     <row r="111" spans="1:8">
       <c r="A111" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B111" s="1">
         <v>384307</v>
@@ -2667,7 +2664,7 @@
     </row>
     <row r="112" spans="1:8">
       <c r="A112" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B112" s="3">
         <v>852075.01370000001</v>
@@ -2684,7 +2681,7 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B113" s="2">
         <f>B111/B112</f>
@@ -2728,7 +2725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>

</xml_diff>